<commit_message>
Improved map graph and fixed bugs
</commit_message>
<xml_diff>
--- a/OECD_Data.xlsx
+++ b/OECD_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dom\Dev\Newcastle\CSC3833\W1\coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942D7516-DDB9-4318-B95E-00678EE208AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8639A846-C090-4C5A-93D8-1F5D0D786315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,9 +219,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>OECD - Total</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>United States of America</t>
   </si>
 </sst>
 </file>
@@ -270,26 +270,26 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -422,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -455,6 +455,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -779,181 +782,181 @@
   </sheetPr>
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="88.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="44.4" customHeight="1">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="88.5" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="E2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="O2" s="14" t="s">
+      <c r="X2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="19.5" customHeight="1">
@@ -2511,7 +2514,7 @@
         <v>14.83</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="14.4" customHeight="1">
+    <row r="24" spans="1:25" ht="19.5" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -2586,7 +2589,7 @@
       </c>
       <c r="Y24" s="6"/>
     </row>
-    <row r="25" spans="1:25" ht="14.4" customHeight="1">
+    <row r="25" spans="1:25" ht="19.5" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>47</v>
       </c>
@@ -2659,7 +2662,7 @@
       </c>
       <c r="Y25" s="4"/>
     </row>
-    <row r="26" spans="1:25" ht="18.75" customHeight="1">
+    <row r="26" spans="1:25" ht="19.5" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -2734,7 +2737,7 @@
       </c>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" ht="14.4" customHeight="1">
+    <row r="27" spans="1:25" ht="19.5" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>49</v>
       </c>
@@ -2807,7 +2810,7 @@
       </c>
       <c r="Y27" s="4"/>
     </row>
-    <row r="28" spans="1:25" ht="14.4" customHeight="1">
+    <row r="28" spans="1:25" ht="19.5" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>50</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>15.45</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="18.75" customHeight="1">
+    <row r="29" spans="1:25" ht="19.5" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>51</v>
       </c>
@@ -2959,7 +2962,7 @@
         <v>14.87</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="18.75" customHeight="1">
+    <row r="30" spans="1:25" ht="19.5" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
@@ -3036,7 +3039,7 @@
         <v>15.67</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="14.4" customHeight="1">
+    <row r="31" spans="1:25" ht="19.5" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>53</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>14.68</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="14.4" customHeight="1">
+    <row r="32" spans="1:25" ht="19.5" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
@@ -3188,7 +3191,7 @@
       </c>
       <c r="Y32" s="6"/>
     </row>
-    <row r="33" spans="1:25" ht="14.4" customHeight="1">
+    <row r="33" spans="1:25" ht="19.5" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -3263,7 +3266,7 @@
       </c>
       <c r="Y33" s="4"/>
     </row>
-    <row r="34" spans="1:25" ht="18.75" customHeight="1">
+    <row r="34" spans="1:25" ht="19.5" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
@@ -3338,7 +3341,7 @@
       </c>
       <c r="Y34" s="6"/>
     </row>
-    <row r="35" spans="1:25" ht="18.75" customHeight="1">
+    <row r="35" spans="1:25" ht="19.5" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -3413,7 +3416,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="14.4" customHeight="1">
+    <row r="36" spans="1:25" ht="19.5" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>58</v>
       </c>
@@ -3486,7 +3489,7 @@
       </c>
       <c r="Y36" s="6"/>
     </row>
-    <row r="37" spans="1:25" ht="18.75" customHeight="1">
+    <row r="37" spans="1:25" ht="19.5" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>59</v>
       </c>
@@ -3557,7 +3560,7 @@
       </c>
       <c r="Y37" s="4"/>
     </row>
-    <row r="38" spans="1:25" ht="14.4" customHeight="1">
+    <row r="38" spans="1:25" ht="19.5" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>60</v>
       </c>
@@ -3628,7 +3631,7 @@
         <v>14.61</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="14.4" customHeight="1">
+    <row r="39" spans="1:25" ht="19.5" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
@@ -3705,9 +3708,9 @@
         <v>14.94</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="14.4" customHeight="1">
+    <row r="40" spans="1:25" ht="19.5" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B40" s="6">
         <v>0.1</v>
@@ -3782,9 +3785,9 @@
         <v>14.57</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="18.75" customHeight="1">
+    <row r="41" spans="1:25" ht="19.5" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="5">
         <v>3</v>
@@ -3859,9 +3862,9 @@
         <v>15.07</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="18.75" customHeight="1">
+    <row r="42" spans="1:25" ht="20.25" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="6">
         <v>6.7</v>
@@ -3918,9 +3921,9 @@
       </c>
       <c r="Y42" s="6"/>
     </row>
-    <row r="43" spans="1:25" ht="14.4" customHeight="1">
+    <row r="43" spans="1:25" ht="19.5" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="4">
         <v>13.8</v>
@@ -3985,9 +3988,9 @@
       </c>
       <c r="Y43" s="4"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" ht="19.5" customHeight="1">
       <c r="A44" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44" s="6">
         <v>35.9</v>
@@ -4046,6 +4049,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add single comparison scatter plot
</commit_message>
<xml_diff>
--- a/OECD_Data.xlsx
+++ b/OECD_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dom\Dev\Newcastle\CSC3833\W1\coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8639A846-C090-4C5A-93D8-1F5D0D786315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADF6DF1-3922-4C9B-B3EC-ACD4B928A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -783,7 +783,7 @@
   <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>